<commit_message>
change of id label in karmen DD
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_KARMEN_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_KARMEN_TRACY.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\Tracy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4690A213-85B2-4516-A8E7-DC9754B9DBF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002CB72E-EE22-4924-AD9A-0961B0CECE88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11340" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>ID of the participant</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
@@ -83,13 +80,16 @@
   </si>
   <si>
     <t>postmenopausal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,14 +116,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -175,18 +167,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,21 +491,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="3"/>
-    <col min="2" max="2" width="26.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="5"/>
+    <col min="1" max="1" width="11.44140625" style="3"/>
+    <col min="2" max="2" width="26.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -529,46 +519,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="B3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="D3" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4"/>
       <c r="B4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>13</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5"/>
       <c r="B5" s="7" t="s">
         <v>5</v>
@@ -580,541 +566,541 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
       <c r="D34"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
       <c r="D35"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
       <c r="D39"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
       <c r="D41"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
       <c r="D42"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
       <c r="D43"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
       <c r="D44"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
       <c r="D45"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
       <c r="D46"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
       <c r="D47"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50"/>
       <c r="D50"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
       <c r="D53"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
       <c r="D57"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
       <c r="D59"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
       <c r="D62"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
       <c r="D63"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>
       <c r="D64"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65"/>
       <c r="D65"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66"/>
       <c r="D66"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67"/>
       <c r="D67"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68"/>
       <c r="B68"/>
       <c r="C68"/>
       <c r="D68"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69"/>
       <c r="D69"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70"/>
       <c r="D70"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71"/>
       <c r="B71"/>
       <c r="C71"/>
       <c r="D71"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72"/>
       <c r="D72"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73"/>
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76"/>
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77"/>
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78"/>
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79"/>
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80"/>
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81"/>
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82"/>
       <c r="B82"/>
       <c r="C82"/>
       <c r="D82"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83"/>
       <c r="B83"/>
       <c r="C83"/>
       <c r="D83"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84"/>
       <c r="B84"/>
       <c r="C84"/>
       <c r="D84"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85"/>
       <c r="B85"/>
       <c r="C85"/>
       <c r="D85"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86"/>
       <c r="B86"/>
       <c r="C86"/>
       <c r="D86"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87"/>
       <c r="B87"/>
       <c r="C87"/>
       <c r="D87"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88"/>
       <c r="B88"/>
       <c r="C88"/>
       <c r="D88"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89"/>
       <c r="D89"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90"/>
       <c r="D90"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91"/>
       <c r="B91"/>
       <c r="C91"/>
       <c r="D91"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92"/>
       <c r="D92"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93"/>
       <c r="B93"/>
       <c r="C93"/>
       <c r="D93"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94"/>
     </row>
   </sheetData>
@@ -1131,14 +1117,14 @@
       <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="3"/>
-    <col min="3" max="3" width="30.5703125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="3"/>
+    <col min="3" max="3" width="30.5546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1150,48 +1136,48 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6">
         <v>2</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="6">
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>18</v>
+      <c r="C5" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1200,12 +1186,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1450,21 +1439,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1489,18 +1484,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ID label change to ID as suggested by Benedikt
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_KARMEN_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_KARMEN_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002CB72E-EE22-4924-AD9A-0961B0CECE88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B6C0F9-EC5C-49B3-9587-FFC7C96D5D17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11340" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
@@ -494,18 +494,18 @@
   <dimension ref="A1:D94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="3"/>
-    <col min="2" max="2" width="26.33203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="5"/>
+    <col min="1" max="1" width="11.42578125" style="3"/>
+    <col min="2" max="2" width="26.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
         <v>7</v>
       </c>
@@ -530,7 +530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="8" t="s">
         <v>9</v>
@@ -542,7 +542,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4" s="8" t="s">
         <v>11</v>
@@ -554,7 +554,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" s="7" t="s">
         <v>5</v>
@@ -566,7 +566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
         <v>13</v>
@@ -578,529 +578,529 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
       <c r="D34"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
       <c r="D35"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
       <c r="D39"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
       <c r="D41"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
       <c r="D42"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
       <c r="D43"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
       <c r="D44"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
       <c r="D45"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
       <c r="D46"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
       <c r="D47"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50"/>
       <c r="D50"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
       <c r="D53"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
       <c r="D57"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
       <c r="D59"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
       <c r="D62"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
       <c r="D63"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>
       <c r="D64"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65"/>
       <c r="D65"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66"/>
       <c r="D66"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67"/>
       <c r="D67"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68"/>
       <c r="B68"/>
       <c r="C68"/>
       <c r="D68"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69"/>
       <c r="D69"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70"/>
       <c r="D70"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71"/>
       <c r="B71"/>
       <c r="C71"/>
       <c r="D71"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72"/>
       <c r="D72"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73"/>
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76"/>
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77"/>
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78"/>
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79"/>
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80"/>
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81"/>
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82"/>
       <c r="B82"/>
       <c r="C82"/>
       <c r="D82"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83"/>
       <c r="B83"/>
       <c r="C83"/>
       <c r="D83"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84"/>
       <c r="B84"/>
       <c r="C84"/>
       <c r="D84"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85"/>
       <c r="B85"/>
       <c r="C85"/>
       <c r="D85"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86"/>
       <c r="B86"/>
       <c r="C86"/>
       <c r="D86"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87"/>
       <c r="B87"/>
       <c r="C87"/>
       <c r="D87"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88"/>
       <c r="B88"/>
       <c r="C88"/>
       <c r="D88"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89"/>
       <c r="D89"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90"/>
       <c r="D90"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91"/>
       <c r="B91"/>
       <c r="C91"/>
       <c r="D91"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92"/>
       <c r="D92"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93"/>
       <c r="B93"/>
       <c r="C93"/>
       <c r="D93"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94"/>
     </row>
   </sheetData>
@@ -1114,17 +1114,17 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C5"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="3"/>
-    <col min="3" max="3" width="30.5546875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="3"/>
+    <col min="3" max="3" width="30.5703125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
@@ -1198,6 +1198,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -1438,15 +1447,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
@@ -1465,6 +1465,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{607F74A7-32EE-406C-A688-0D84C4E12BE8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1481,12 +1489,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>